<commit_message>
primary effort for adding financing
current_step cannot be used
</commit_message>
<xml_diff>
--- a/run_sheets/duopoly_heterogeneous_wcap.xlsx
+++ b/run_sheets/duopoly_heterogeneous_wcap.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="2">
         <v>5.7</v>
@@ -481,7 +481,7 @@
         <v>2E-3</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="D3" s="2">
         <v>5.7</v>
@@ -516,7 +516,7 @@
         <v>2E-3</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="D4" s="3">
         <v>5.4</v>
@@ -551,7 +551,7 @@
         <v>2E-3</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="D5" s="3">
         <v>5.4</v>
@@ -586,7 +586,7 @@
         <v>2E-3</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -597,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="D6" s="3">
         <v>5.0999999999999996</v>
@@ -621,7 +621,7 @@
         <v>2E-3</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>600</v>
+        <v>6000</v>
       </c>
       <c r="D7" s="3">
         <v>5.0999999999999996</v>
@@ -656,7 +656,7 @@
         <v>2E-3</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>